<commit_message>
read-only access is given for excel test file
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/dataset/Monthly_Data_Query.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/dataset/Monthly_Data_Query.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="23040" windowHeight="8415"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="23040" windowHeight="8415"/>
   </bookViews>
   <sheets>
     <sheet name="Monthly_Data_Query" sheetId="1" r:id="rId1"/>
@@ -1820,7 +1820,7 @@
   <dimension ref="A1:KC115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>